<commit_message>
Verificación CMMI-Inicio de Sesión
version 0.2
consulta de dispositivos
</commit_message>
<xml_diff>
--- a/Verificación CMMI-Inicio de Sesión.xlsx
+++ b/Verificación CMMI-Inicio de Sesión.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ADSI\A-Proyecto\Gestión de Calidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aprendíz\Documents\GitHub\ProyectoCis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Cumple</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>¿El sistema indica si el usuario ya está registrado?</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>consulta en que dispositivos se inicio sesion con anterioridad</t>
   </si>
 </sst>
 </file>
@@ -527,7 +533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -773,7 +781,9 @@
         <v>25</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -785,11 +795,15 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>

</xml_diff>